<commit_message>
UseManager에 값 추가(name, userType, accountType) API 일부 수정
</commit_message>
<xml_diff>
--- a/Document/API.xlsx
+++ b/Document/API.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LimHJ\Desktop\Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lim HJ\Desktop\소마\과제\BlockBuster\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="173">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -207,10 +207,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>나중에 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Integer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -684,6 +680,42 @@
   </si>
   <si>
     <t>previous_rank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오류 없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accountType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정 타입</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -779,7 +811,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -844,6 +876,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1160,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:G20"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1176,7 +1220,7 @@
     <col min="6" max="6" width="11.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="38" style="3" customWidth="1"/>
     <col min="8" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="9" style="1"/>
+    <col min="9" max="9" width="13.75" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.875" style="1" customWidth="1"/>
     <col min="11" max="12" width="9" style="1"/>
     <col min="13" max="13" width="31.875" style="3" customWidth="1"/>
@@ -1214,18 +1258,24 @@
       <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="O1">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="18">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="22" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1255,14 +1305,14 @@
         <v>101</v>
       </c>
       <c r="P2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
       <c r="E3" s="8" t="s">
         <v>19</v>
       </c>
@@ -1290,14 +1340,14 @@
         <v>102</v>
       </c>
       <c r="P3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1316,14 +1366,14 @@
         <v>103</v>
       </c>
       <c r="P4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="10" t="s">
         <v>15</v>
       </c>
@@ -1345,30 +1395,30 @@
         <v>104</v>
       </c>
       <c r="P5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="18">
+      <c r="A6" s="22">
         <v>2</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="18" t="s">
-        <v>143</v>
+      <c r="D6" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>17</v>
@@ -1388,14 +1438,14 @@
         <v>200</v>
       </c>
       <c r="P6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="10" t="s">
         <v>34</v>
       </c>
@@ -1423,551 +1473,517 @@
         <v>201</v>
       </c>
       <c r="P7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="18">
+      <c r="A8" s="22">
         <v>3</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E8" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="L8" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="M8" s="3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="O8">
         <v>500</v>
       </c>
       <c r="P8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>47</v>
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="9"/>
+      <c r="I9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>170</v>
       </c>
       <c r="O9">
         <v>501</v>
       </c>
       <c r="P9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="18">
-        <v>4</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
       <c r="I10" s="1" t="s">
-        <v>26</v>
+        <v>166</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="O10">
         <v>502</v>
       </c>
       <c r="P10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>130</v>
-      </c>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
       <c r="I11" s="1" t="s">
-        <v>79</v>
+        <v>167</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>40</v>
+        <v>172</v>
       </c>
       <c r="O11">
         <v>600</v>
       </c>
       <c r="P11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="18">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <v>4</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
         <v>5</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B15" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="D15" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="E15" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="G12" s="14" t="s">
+      <c r="F16" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="22">
+        <v>6</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="22">
+        <v>7</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="F22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8" t="s">
+      <c r="L22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="22">
+        <v>8</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="M13" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="18">
-        <v>6</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" s="2" t="s">
+      <c r="G24" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="L24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="M18" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="18">
-        <v>7</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="18" t="s">
+      <c r="M24" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="M20" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="18">
-        <v>8</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="M22" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
-        <v>9</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>104</v>
-      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="13"/>
       <c r="H25" s="12"/>
       <c r="I25" s="10" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -1975,39 +1991,104 @@
         <v>38</v>
       </c>
       <c r="M25" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="22">
+        <v>9</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M28" s="13" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="D15:D18"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D5"/>
@@ -2016,6 +2097,30 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="C18:C21"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2027,7 +2132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2043,24 +2148,24 @@
   <sheetData>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" t="s">
         <v>160</v>
-      </c>
-      <c r="G5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2068,37 +2173,37 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2106,31 +2211,31 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2149,52 +2254,52 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API 수정 (Login할 때 name, accountType, userType도 추가로 보냄)
</commit_message>
<xml_diff>
--- a/Document/API.xlsx
+++ b/Document/API.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="177">
   <si>
     <t>API</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -259,6 +259,342 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인한 유저의 uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인한 유저의 sid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Integer </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>에러 코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결과 전송</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저의 uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>얻은 Score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isNewRecord</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rankChange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 기록이 새로운 기록인가?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순위 변동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그아웃할 유저의 uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결과(성공시 True)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의 순위 가져옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1/score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1/user/logout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의 순위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순위들 가져옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1/score/all</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rankStart</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rankEnd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순위들을 가져올 시작점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순위들을 가져올 끝점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data(list)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 순위의 유저의 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 순위의 점수(내림차순)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>join_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>access_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>last_play_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(40)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INTEGER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Log_Score</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 조회(uid)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1/user/uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 조회(기타)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/api/v1/user/etc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>찾을 유저의 계정 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>찾을 유저의 이메일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결과(있으면 True)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>account_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(15)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(15)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 Facebook으로 계정이 이미 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 Twitter로 계정이 이미 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 Google로 계정이 이미 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 Email로 계정이 이미 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당하는 uid에 맞는 계정이 없습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당하는 기타 정보에 맞는 계정이 없습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>sid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -267,27 +603,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>로그인한 유저의 uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그인한 유저의 sid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Integer </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>에러 코드</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결과 전송</t>
+    <t>로그아웃할 유저의 sid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>순위를 가져올 유저의 uid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accountType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저의 계정 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해당 계정이 없습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호가 맞지 않습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미 접속해 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저의 sid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세션 인증 실패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Log_Access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(40)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(40)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHAR(40)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>INTEGER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>previous_rank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오류 없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accountType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유저 타입</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계정 타입</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -295,135 +719,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유저의 uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>얻은 Score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>isNewRecord</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rankChange</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이 기록이 새로운 기록인가?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>순위</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>순위 변동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그아웃</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그아웃할 유저의 uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Integer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결과(성공시 True)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나의 순위 가져옴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1/score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1/user/logout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>나의 순위</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>순위들 가져옴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1/score/all</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rankStart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>rankEnd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>순위들을 가져올 시작점</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>순위들을 가져올 끝점</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>data(list)</t>
+    <t>sid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결과(있으면 True)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -431,291 +731,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당 순위의 유저의 이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당 순위의 점수(내림차순)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>User</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>join_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>access_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>last_play_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(50)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(40)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INTEGER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Log_Score</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DATETIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DATETIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DATETIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DATETIME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>close_date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 조회(uid)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1/user/uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>회원 조회(기타)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/api/v1/user/etc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>찾을 유저의 계정 타입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>찾을 유저의 이메일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>결과(있으면 True)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>user_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>account_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(15)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(15)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당 Facebook으로 계정이 이미 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당 Twitter로 계정이 이미 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당 Google로 계정이 이미 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당 Email로 계정이 이미 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당하는 uid에 맞는 계정이 없습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당하는 기타 정보에 맞는 계정이 없습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PUT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>로그아웃할 유저의 sid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>순위를 가져올 유저의 uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>accountType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유저의 계정 타입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>해당 계정이 없습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>비밀번호가 맞지 않습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이미 접속해 있습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유저의 sid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>세션 인증 실패</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Log_Access</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(40)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(40)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VARCHAR(40)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INTEGER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>previous_rank</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오류 없음</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>userType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>accountType</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이름</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>유저 타입</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>계정 타입</t>
+    <t>로그인한 유저의 이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -811,7 +827,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -856,15 +872,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1204,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="E12" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1262,20 +1269,20 @@
         <v>0</v>
       </c>
       <c r="P1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="22">
+      <c r="A2" s="19">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="19" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1305,14 +1312,14 @@
         <v>101</v>
       </c>
       <c r="P2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
       <c r="E3" s="8" t="s">
         <v>19</v>
       </c>
@@ -1340,14 +1347,14 @@
         <v>102</v>
       </c>
       <c r="P3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="8" t="s">
         <v>14</v>
       </c>
@@ -1366,14 +1373,14 @@
         <v>103</v>
       </c>
       <c r="P4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="10" t="s">
         <v>15</v>
       </c>
@@ -1395,21 +1402,21 @@
         <v>104</v>
       </c>
       <c r="P5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="22">
+      <c r="A6" s="19">
         <v>2</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>142</v>
+      <c r="D6" s="19" t="s">
+        <v>141</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>55</v>
@@ -1438,14 +1445,14 @@
         <v>200</v>
       </c>
       <c r="P6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
       <c r="E7" s="10" t="s">
         <v>34</v>
       </c>
@@ -1473,26 +1480,26 @@
         <v>201</v>
       </c>
       <c r="P7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="19">
         <v>3</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="18" t="s">
+      <c r="E8" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="15" t="s">
         <v>42</v>
       </c>
       <c r="G8" s="14" t="s">
@@ -1514,82 +1521,82 @@
         <v>500</v>
       </c>
       <c r="P8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
       <c r="G9" s="9"/>
       <c r="I9" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="O9">
         <v>501</v>
       </c>
       <c r="P9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="I10" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O10">
         <v>502</v>
       </c>
       <c r="P10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
       <c r="I11" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="M11" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O11">
         <v>600</v>
       </c>
       <c r="P11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="13"/>
       <c r="H12" s="12"/>
       <c r="I12" s="10" t="s">
@@ -1605,62 +1612,62 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+      <c r="A13" s="22">
         <v>4</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="D13" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="E13" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="I13" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21" t="s">
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>131</v>
-      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="21" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="21" t="s">
-        <v>59</v>
+      <c r="F14" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18" t="s">
         <v>29</v>
       </c>
       <c r="M14" s="3" t="s">
@@ -1668,26 +1675,26 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="22">
+      <c r="A15" s="19">
         <v>5</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="19" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>149</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>150</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>54</v>
@@ -1695,396 +1702,481 @@
       <c r="I15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="17" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>51</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="I16" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M16" s="9" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="16" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>64</v>
+      <c r="H17" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="22">
-        <v>6</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
       <c r="I18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>28</v>
+        <v>167</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>75</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>74</v>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="9"/>
+      <c r="I19" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18" t="s">
+        <v>168</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>76</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>74</v>
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="9"/>
+      <c r="I20" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18" t="s">
+        <v>167</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>77</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="13"/>
       <c r="H21" s="12"/>
       <c r="I21" s="10" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
       <c r="L21" s="10" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="M21" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="19">
+        <v>6</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="22">
-        <v>7</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>51</v>
+      <c r="C22" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="L22" s="1" t="s">
-        <v>37</v>
+      <c r="J22" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="10" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="F23" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="H23" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>46</v>
+      <c r="G23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="22">
-        <v>8</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>59</v>
+      <c r="F24" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>38</v>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18" t="s">
+        <v>73</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
       <c r="G25" s="13"/>
       <c r="H25" s="12"/>
-      <c r="I25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10" t="s">
-        <v>38</v>
+      <c r="I25" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="22">
-        <v>9</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>93</v>
+      <c r="A26" s="19">
+        <v>7</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>79</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="19">
+        <v>8</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="M29" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" s="19">
+        <v>9</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K26" s="1" t="s">
+      <c r="L30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M26" s="3" t="s">
+      <c r="L31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M31" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M27" s="3" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="10" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10" t="s">
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M28" s="13" t="s">
+      <c r="M32" s="13" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="D22:D25"/>
+    <mergeCell ref="B15:B21"/>
+    <mergeCell ref="A15:A21"/>
+    <mergeCell ref="C15:C21"/>
+    <mergeCell ref="D15:D21"/>
     <mergeCell ref="A8:A12"/>
     <mergeCell ref="B8:B12"/>
     <mergeCell ref="C8:C12"/>
@@ -2097,30 +2189,22 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="C18:C21"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2148,24 +2232,24 @@
   <sheetData>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" t="s">
         <v>159</v>
-      </c>
-      <c r="G5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -2173,37 +2257,37 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2211,31 +2295,31 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2254,52 +2338,52 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>